<commit_message>
find a helpline added & module code generator included in directory.
</commit_message>
<xml_diff>
--- a/data-raw/Rolodex.xlsx
+++ b/data-raw/Rolodex.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\ModuleTest\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\Rolodex\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A5FF76-1DF7-47A1-9B35-8D788CC79120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA0111E-4921-4FF4-89EF-022B11FDBBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="17820" windowHeight="11210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="480" windowWidth="17820" windowHeight="11210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rolodex NEW" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="371">
   <si>
     <t>Name</t>
   </si>
@@ -1145,12 +1145,43 @@
   <si>
     <t>National Gambler Support Line</t>
   </si>
+  <si>
+    <t>Find a Helpline</t>
+  </si>
+  <si>
+    <t>https://findahelpline.com/i/iasp</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Find a wide variety of FREE helplines available in the US. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>CATEGORIES</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: Abuse &amp; Domestic Violence; Anxiety; Bullying; Depression; Eating &amp; Body Image; Family; Gambling; Gender &amp; Sexual Identity; Grief &amp; Loss; Loneliness; Physical illness; Pregnancy &amp; Abortion; Relationships; School &amp; Work; Self-harm; Sexual abuse; Stress; Substance use; Suicidal thoughts; Supporting others; Trauma &amp; PTSD</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1315,6 +1346,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0C0C0C"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -2029,10 +2068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="G80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4438,6 +4477,23 @@
       </c>
       <c r="I95" s="1" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added international hotline text
</commit_message>
<xml_diff>
--- a/data-raw/Rolodex.xlsx
+++ b/data-raw/Rolodex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\Rolodex\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA0111E-4921-4FF4-89EF-022B11FDBBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782CEF6B-1DA9-48A8-A580-68D71658F309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="480" windowWidth="17820" windowHeight="11210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1153,7 +1153,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Find a wide variety of FREE helplines available in the US. </t>
+      <t xml:space="preserve">Find a wide variety of FREE helplines available in the US and Internationally. </t>
     </r>
     <r>
       <rPr>
@@ -2071,7 +2071,7 @@
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I92" sqref="I92"/>
+      <selection activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
New OASAS Champ Program Added to MH and AOD
</commit_message>
<xml_diff>
--- a/data-raw/Rolodex.xlsx
+++ b/data-raw/Rolodex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\New Shiny Apps\Rolodex\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72DB112-927E-428B-B933-155ADAF00A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFA5BFD-A3B6-48D5-992C-7AD89481549F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rolodex NEW" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="505">
   <si>
     <t>Name</t>
   </si>
@@ -1461,9 +1461,6 @@
     <t>https://www.facebook.com/groups/694681097335282/</t>
   </si>
   <si>
-    <t>Physical</t>
-  </si>
-  <si>
     <t>A community of black girls and women to encourage physical activity and promote health through running and/or walking with every level of fitness welcomed</t>
   </si>
   <si>
@@ -1493,9 +1490,6 @@
   </si>
   <si>
     <t xml:space="preserve">All paces welcomed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Albany Running Exchange </t>
   </si>
   <si>
     <t>Where/When: Monday-Sunday, location varies</t>
@@ -1583,6 +1577,35 @@
   </si>
   <si>
     <t>St. Vincent De Paul Food Pantry</t>
+  </si>
+  <si>
+    <t>Albany Running Exchange</t>
+  </si>
+  <si>
+    <t>ombuds@oasas.ny.gov</t>
+  </si>
+  <si>
+    <t>M-W 9am-7pm - Th-F 9am-4pm</t>
+  </si>
+  <si>
+    <t>https://www.cssny.org/programs/entry/champ</t>
+  </si>
+  <si>
+    <t>CHAMP Program (OASAS)</t>
+  </si>
+  <si>
+    <t>tel:8886145400</t>
+  </si>
+  <si>
+    <t>Have questions about mental health or substance use health insurance?
+The OASAS CHAMP program can help:
+Teach you about your insurance rights
+Find the best insurance option
+Access coverage for treatment and medication
+Advocate with providers and insurance companies
+Submit complaints against insurance companies
+Fight denials and file appeals
+New York State Office of Addiction Services and Supports (OASAS)</t>
   </si>
 </sst>
 </file>
@@ -2138,7 +2161,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2177,6 +2200,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2533,10 +2557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G125" sqref="G125"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2575,86 +2599,82 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>133</v>
+        <v>502</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>134</v>
+        <v>500</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>499</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>276</v>
+        <v>502</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="22" t="s">
+        <v>503</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
+        <v>501</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>499</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>174</v>
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>132</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>34</v>
+        <v>133</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>32</v>
@@ -2663,27 +2683,27 @@
         <v>26</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>177</v>
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>337</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
@@ -2692,25 +2712,27 @@
         <v>26</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>277</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>32</v>
@@ -2719,25 +2741,27 @@
         <v>26</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>177</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>32</v>
@@ -2746,12 +2770,12 @@
         <v>26</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>270</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>144</v>
@@ -2760,11 +2784,11 @@
         <v>279</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>32</v>
@@ -2773,27 +2797,25 @@
         <v>26</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>180</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>32</v>
@@ -2802,77 +2824,97 @@
         <v>26</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>181</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>383</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="1" t="s">
-        <v>389</v>
-      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="11" t="s">
-        <v>390</v>
+      <c r="I12" s="1" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="C13" s="9"/>
+        <v>384</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>383</v>
+      </c>
       <c r="D13" s="1" t="s">
-        <v>386</v>
+        <v>51</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>52</v>
@@ -2880,95 +2922,86 @@
       <c r="H13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I13" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3" t="s">
-        <v>335</v>
-      </c>
+        <v>388</v>
+      </c>
+      <c r="C14" s="9"/>
       <c r="D14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1" t="s">
-        <v>55</v>
+        <v>389</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>282</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="C15" s="9"/>
       <c r="D15" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+        <v>386</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>185</v>
+      <c r="I15" s="10" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>323</v>
+        <v>53</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="3" t="s">
+        <v>335</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="G16" s="1" t="s">
         <v>52</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>339</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
         <v>52</v>
       </c>
@@ -2976,70 +3009,57 @@
         <v>10</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>340</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>136</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>283</v>
+        <v>153</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>323</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>58</v>
+        <v>338</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>339</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>190</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>138</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>144</v>
@@ -3063,12 +3083,12 @@
         <v>26</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>144</v>
@@ -3092,12 +3112,12 @@
         <v>26</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>144</v>
@@ -3121,85 +3141,85 @@
         <v>26</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>312</v>
+        <v>283</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>194</v>
+        <v>177</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>65</v>
+        <v>284</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>312</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>62</v>
@@ -3208,25 +3228,27 @@
         <v>26</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="F26" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>62</v>
@@ -3235,61 +3257,74 @@
         <v>26</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>271</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>350</v>
+        <v>63</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>351</v>
+        <v>62</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>352</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>212</v>
+        <v>66</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G28" s="1" t="s">
-        <v>351</v>
+        <v>62</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>213</v>
+        <v>271</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>354</v>
+        <v>349</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>350</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>351</v>
@@ -3298,32 +3333,41 @@
         <v>10</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>357</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
         <v>351</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I30" s="7" t="s">
-        <v>358</v>
+      <c r="I30" s="1" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>360</v>
+        <v>366</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>354</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>351</v>
@@ -3331,103 +3375,81 @@
       <c r="H31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I31" s="8" t="s">
-        <v>361</v>
+      <c r="I31" s="1" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>362</v>
+      <c r="A32" s="1" t="s">
+        <v>356</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="G32" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>365</v>
+      <c r="H32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>359</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>360</v>
+      </c>
       <c r="G33" s="1" t="s">
-        <v>71</v>
+        <v>351</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I33" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H34" s="1" t="s">
+      <c r="I33" s="8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>202</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
         <v>71</v>
       </c>
@@ -3435,24 +3457,28 @@
         <v>10</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>332</v>
+        <v>156</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G36" s="1" t="s">
         <v>71</v>
       </c>
@@ -3460,27 +3486,25 @@
         <v>10</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>71</v>
@@ -3489,25 +3513,23 @@
         <v>10</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>159</v>
+        <v>19</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>332</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>207</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
         <v>71</v>
@@ -3516,94 +3538,104 @@
         <v>10</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>150</v>
+        <v>167</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>76</v>
+        <v>205</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>209</v>
+        <v>72</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>71</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B40" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="C40" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E40" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="G41" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -3614,23 +3646,21 @@
         <v>10</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B43" s="1"/>
-      <c r="C43" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>226</v>
-      </c>
+      <c r="C43" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
         <v>79</v>
@@ -3639,19 +3669,19 @@
         <v>10</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>169</v>
+        <v>81</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>83</v>
+        <v>215</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -3662,19 +3692,24 @@
         <v>10</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>366</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B45" s="1"/>
       <c r="C45" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>354</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
         <v>79</v>
       </c>
@@ -3682,264 +3717,259 @@
         <v>10</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>355</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>328</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="B46" s="1"/>
       <c r="C46" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>28</v>
+        <v>294</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+        <v>366</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>354</v>
+      </c>
       <c r="G47" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>273</v>
+        <v>355</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>8</v>
+        <v>141</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>159</v>
+        <v>328</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>207</v>
-      </c>
+        <v>329</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>272</v>
+        <v>219</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>87</v>
+        <v>27</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>333</v>
       </c>
       <c r="E49" s="1"/>
-      <c r="F49" s="1" t="s">
-        <v>223</v>
-      </c>
+      <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>90</v>
+        <v>290</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>91</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
         <v>86</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>225</v>
+        <v>272</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>151</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="B51" s="1"/>
       <c r="C51" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>228</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" s="1"/>
       <c r="F51" s="1" t="s">
-        <v>94</v>
+        <v>223</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>86</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>344</v>
+        <v>89</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>86</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>342</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>345</v>
+        <v>92</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>86</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>346</v>
+        <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B54" s="1"/>
-      <c r="C54" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
+        <v>343</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>344</v>
+      </c>
       <c r="G54" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>229</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
+        <v>347</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>345</v>
+      </c>
       <c r="G55" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>232</v>
+        <v>346</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="3" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>99</v>
+        <v>315</v>
       </c>
       <c r="E56" s="1"/>
-      <c r="F56" s="4" t="s">
-        <v>230</v>
-      </c>
+      <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
         <v>96</v>
       </c>
@@ -3947,19 +3977,19 @@
         <v>10</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>324</v>
+        <v>97</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3970,22 +4000,24 @@
         <v>10</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="3" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>309</v>
+        <v>99</v>
       </c>
       <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="F58" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="G58" s="1" t="s">
         <v>96</v>
       </c>
@@ -3993,19 +4025,19 @@
         <v>10</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>100</v>
+        <v>324</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>234</v>
+        <v>313</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -4016,19 +4048,19 @@
         <v>10</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -4039,19 +4071,19 @@
         <v>10</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -4062,19 +4094,19 @@
         <v>10</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -4085,19 +4117,19 @@
         <v>10</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>318</v>
+        <v>238</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -4108,19 +4140,19 @@
         <v>10</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>104</v>
+        <v>22</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -4131,67 +4163,67 @@
         <v>10</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>299</v>
+        <v>103</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="3" t="s">
+        <v>281</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="3" t="s">
-        <v>281</v>
+        <v>114</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>299</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>107</v>
+        <v>311</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -4202,19 +4234,19 @@
         <v>10</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -4225,19 +4257,19 @@
         <v>10</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>321</v>
+        <v>107</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -4248,19 +4280,19 @@
         <v>10</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>111</v>
+        <v>320</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -4271,19 +4303,19 @@
         <v>10</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>113</v>
+        <v>321</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -4294,19 +4326,19 @@
         <v>10</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>238</v>
+        <v>111</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -4317,19 +4349,19 @@
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="3" t="s">
         <v>281</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>317</v>
+        <v>113</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -4340,80 +4372,74 @@
         <v>10</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>330</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B74" s="1"/>
       <c r="C74" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>161</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B75" s="1"/>
       <c r="C75" s="3" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>250</v>
+        <v>317</v>
       </c>
       <c r="E75" s="1"/>
-      <c r="F75" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>162</v>
+        <v>330</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+        <v>300</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="G76" s="1" t="s">
         <v>115</v>
       </c>
@@ -4421,24 +4447,26 @@
         <v>10</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>325</v>
+        <v>116</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>327</v>
+        <v>301</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
+      <c r="F77" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="G77" s="1" t="s">
         <v>115</v>
       </c>
@@ -4446,25 +4474,23 @@
         <v>10</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>303</v>
+        <v>162</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>257</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
         <v>115</v>
@@ -4473,21 +4499,21 @@
         <v>10</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>120</v>
+        <v>325</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>304</v>
+        <v>326</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>259</v>
+        <v>327</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -4498,23 +4524,25 @@
         <v>10</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>305</v>
+        <v>255</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>303</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E80" s="1"/>
+        <v>256</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
         <v>115</v>
@@ -4523,85 +4551,77 @@
         <v>10</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>274</v>
+        <v>164</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
         <v>115</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
       <c r="G82" s="1" t="s">
         <v>115</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>306</v>
+      <c r="C83" s="5" t="s">
+        <v>274</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>263</v>
+        <v>76</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>264</v>
+        <v>209</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>115</v>
@@ -4610,84 +4630,84 @@
         <v>26</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>265</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>74</v>
+        <v>276</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F84" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="G84" s="1" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>330</v>
+        <v>150</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>300</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>12</v>
+        <v>306</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>220</v>
+        <v>264</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>156</v>
+        <v>8</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
         <v>9</v>
       </c>
@@ -4695,25 +4715,27 @@
         <v>10</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>202</v>
+        <v>272</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>341</v>
-      </c>
-      <c r="E87" s="1"/>
+        <v>330</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="F87" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>9</v>
@@ -4722,24 +4744,28 @@
         <v>10</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>332</v>
+        <v>156</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G88" s="1" t="s">
         <v>9</v>
       </c>
@@ -4747,22 +4773,26 @@
         <v>10</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B89" s="1"/>
-      <c r="C89" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>341</v>
       </c>
       <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
+      <c r="F89" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="G89" s="1" t="s">
         <v>9</v>
       </c>
@@ -4770,19 +4800,21 @@
         <v>10</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B90" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>332</v>
+      </c>
       <c r="C90" s="3" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>23</v>
+        <v>310</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
@@ -4793,50 +4825,42 @@
         <v>10</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>150</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B91" s="1"/>
       <c r="C91" s="3" t="s">
-        <v>306</v>
+        <v>281</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>333</v>
+        <v>22</v>
+      </c>
+      <c r="B92" s="1"/>
+      <c r="C92" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
@@ -4847,24 +4871,28 @@
         <v>10</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>141</v>
+        <v>24</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="C93" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
+        <v>150</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="G93" s="1" t="s">
         <v>9</v>
       </c>
@@ -4872,71 +4900,69 @@
         <v>26</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>219</v>
+        <v>265</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B94" s="1"/>
-      <c r="C94" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>215</v>
+        <v>27</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>333</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>214</v>
+        <v>273</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>266</v>
+        <v>328</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E95" s="1"/>
-      <c r="F95" s="1" t="s">
-        <v>129</v>
-      </c>
+      <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>267</v>
+        <v>219</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>328</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B96" s="1"/>
       <c r="C96" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>28</v>
+        <v>292</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -4944,119 +4970,137 @@
         <v>127</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B97" s="1"/>
+        <v>168</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="C97" s="3" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>83</v>
+        <v>266</v>
       </c>
       <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
+      <c r="F97" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="G97" s="1" t="s">
         <v>127</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>218</v>
+        <v>267</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>166</v>
+        <v>328</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>128</v>
+        <v>329</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E98" s="1"/>
-      <c r="F98" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
         <v>127</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I98" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
+      <c r="G99" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I100" s="1" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A99" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H99" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H100" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I100" s="1" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>10</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="G102" s="3" t="s">
         <v>52</v>
@@ -5065,15 +5109,15 @@
         <v>10</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="G103" s="3" t="s">
         <v>52</v>
@@ -5082,53 +5126,41 @@
         <v>10</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="C104" s="12" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I104" s="7" t="s">
-        <v>394</v>
+      <c r="I104" s="1" t="s">
+        <v>379</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="C105" s="12" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I105" s="7" t="s">
-        <v>394</v>
+      <c r="I105" s="1" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
@@ -5144,8 +5176,8 @@
       <c r="E106" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G106" s="1" t="s">
-        <v>96</v>
+      <c r="G106" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>10</v>
@@ -5167,8 +5199,8 @@
       <c r="E107" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="G107" s="1" t="s">
-        <v>105</v>
+      <c r="G107" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>10</v>
@@ -5191,7 +5223,7 @@
         <v>398</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>10</v>
@@ -5202,172 +5234,160 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>392</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>398</v>
       </c>
       <c r="G109" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H109" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I109" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="G110" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H109" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I109" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A110" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="D110" s="12" t="s">
-        <v>401</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="H110" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I110" s="1" t="s">
-        <v>402</v>
+      <c r="H110" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I110" s="7" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H111" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A113" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="D111" s="3" t="s">
+      <c r="D113" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="E111" s="3" t="s">
+      <c r="E113" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="G111" s="1" t="s">
+      <c r="G113" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="H111" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I111" s="1" t="s">
+      <c r="H113" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I113" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A112" s="3" t="s">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B114" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="C112" s="12" t="s">
+      <c r="C114" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="D112" s="3" t="s">
+      <c r="D114" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="E112" s="3" t="s">
+      <c r="E114" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="F112" s="12" t="s">
+      <c r="F114" s="12" t="s">
         <v>410</v>
       </c>
-      <c r="G112" s="3" t="s">
+      <c r="G114" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H112" s="3" t="s">
+      <c r="H114" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I112" s="13" t="s">
+      <c r="I114" s="13" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="10" t="s">
+    <row r="115" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="B115" s="14" t="s">
         <v>445</v>
       </c>
-      <c r="C113" s="14" t="s">
+      <c r="C115" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="D113" s="14" t="s">
+      <c r="D115" s="14" t="s">
         <v>414</v>
       </c>
-      <c r="E113" s="15" t="s">
+      <c r="E115" s="15" t="s">
         <v>415</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F115" t="s">
         <v>416</v>
-      </c>
-      <c r="G113" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="H113" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I113" s="10" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A114" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="B114" s="14" t="s">
-        <v>420</v>
-      </c>
-      <c r="C114" t="s">
-        <v>421</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="E114" s="15" t="s">
-        <v>422</v>
-      </c>
-      <c r="F114" t="s">
-        <v>423</v>
-      </c>
-      <c r="G114" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="H114" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I114" s="10" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A115" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="B115" s="14" t="s">
-        <v>425</v>
-      </c>
-      <c r="C115" t="s">
-        <v>426</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>427</v>
-      </c>
-      <c r="E115" s="15" t="s">
-        <v>428</v>
-      </c>
-      <c r="F115" t="s">
-        <v>126</v>
       </c>
       <c r="G115" s="14" t="s">
         <v>417</v>
@@ -5376,432 +5396,494 @@
         <v>10</v>
       </c>
       <c r="I115" s="10" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="A116" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="C116" t="s">
+        <v>421</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="E116" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="F116" t="s">
+        <v>423</v>
+      </c>
+      <c r="G116" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="H116" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I116" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="C117" t="s">
+        <v>426</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>427</v>
+      </c>
+      <c r="E117" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="F117" t="s">
+        <v>126</v>
+      </c>
+      <c r="G117" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="H117" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I117" s="10" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A116" s="10" t="s">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A118" s="10" t="s">
         <v>430</v>
       </c>
-      <c r="B116" s="12"/>
-      <c r="C116" s="14"/>
-      <c r="D116" s="14" t="s">
+      <c r="B118" s="12"/>
+      <c r="C118" s="14"/>
+      <c r="D118" s="14" t="s">
         <v>431</v>
       </c>
-      <c r="E116" s="14"/>
-      <c r="F116" s="14"/>
-      <c r="G116" s="1" t="s">
+      <c r="E118" s="14"/>
+      <c r="F118" s="14"/>
+      <c r="G118" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H116" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I116" s="10" t="s">
+      <c r="H118" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I118" s="10" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A117" s="10" t="s">
+    <row r="119" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="A119" s="10" t="s">
         <v>433</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="B119" s="14" t="s">
         <v>434</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C119" t="s">
         <v>435</v>
       </c>
-      <c r="D117" s="14" t="s">
+      <c r="D119" s="14" t="s">
         <v>436</v>
       </c>
-      <c r="E117" s="14" t="s">
+      <c r="E119" s="14" t="s">
         <v>447</v>
       </c>
-      <c r="F117" t="s">
+      <c r="F119" t="s">
         <v>437</v>
       </c>
-      <c r="G117" s="1" t="s">
+      <c r="G119" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H117" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I117" s="10" t="s">
+      <c r="H119" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I119" s="10" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="A118" s="14" t="s">
+    <row r="120" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+      <c r="A120" s="14" t="s">
         <v>439</v>
       </c>
-      <c r="B118" s="14" t="s">
+      <c r="B120" s="14" t="s">
         <v>440</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C120" t="s">
         <v>441</v>
       </c>
-      <c r="D118" s="14" t="s">
+      <c r="D120" s="14" t="s">
         <v>442</v>
       </c>
-      <c r="E118" s="14" t="s">
+      <c r="E120" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="F118" t="s">
+      <c r="F120" t="s">
         <v>443</v>
       </c>
-      <c r="G118" s="14" t="s">
+      <c r="G120" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H118" s="14" t="s">
+      <c r="H120" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I118" s="10" t="s">
+      <c r="I120" s="10" t="s">
         <v>444</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A119" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="C119" s="12" t="s">
-        <v>450</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="E119" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="H119" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I119" s="1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A120" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E120" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="G120" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H120" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I120" s="1" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C121" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I121" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A122" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D122" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="E121" s="3" t="s">
+      <c r="E122" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="G121" s="1" t="s">
+      <c r="G122" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I122" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A123" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="G123" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H121" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I121" s="1" t="s">
+      <c r="H123" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I123" s="1" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="93" x14ac:dyDescent="0.35">
-      <c r="A122" s="16" t="s">
+    <row r="124" spans="1:9" ht="93" x14ac:dyDescent="0.35">
+      <c r="A124" s="16" t="s">
         <v>458</v>
       </c>
-      <c r="B122" s="17" t="s">
+      <c r="B124" s="17" t="s">
         <v>459</v>
       </c>
-      <c r="D122" s="16" t="s">
+      <c r="D124" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="G122" s="16" t="s">
+      <c r="G124" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I124" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="H122" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I122" s="1" t="s">
+    </row>
+    <row r="125" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A125" s="16" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A123" s="16" t="s">
+      <c r="B125" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="D125" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="D123" s="12" t="s">
+      <c r="F125" s="18" t="s">
         <v>465</v>
       </c>
-      <c r="F123" s="18" t="s">
+      <c r="G125" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H125" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I125" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="G123" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="H123" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I123" s="1" t="s">
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A126" s="3" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A124" s="3" t="s">
+      <c r="B126" s="16" t="s">
         <v>468</v>
       </c>
-      <c r="B124" s="16" t="s">
+      <c r="F126" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="F124" s="3" t="s">
+      <c r="G126" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I126" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="G124" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="H124" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I124" s="1" t="s">
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A127" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="B127" s="3" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A125" s="3" t="s">
+      <c r="C127" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="D127" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="C125" s="12" t="s">
+      <c r="F127" s="20" t="s">
         <v>474</v>
       </c>
-      <c r="D125" s="12" t="s">
+      <c r="G127" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H127" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="232.5" x14ac:dyDescent="0.35">
+      <c r="A128" s="19" t="s">
         <v>475</v>
       </c>
-      <c r="F125" s="20" t="s">
+      <c r="B128" s="19" t="s">
         <v>476</v>
       </c>
-      <c r="G125" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="H125" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" ht="232.5" x14ac:dyDescent="0.35">
-      <c r="A126" s="19" t="s">
+      <c r="C128" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="B126" s="19" t="s">
+      <c r="D128" s="16" t="s">
         <v>478</v>
       </c>
-      <c r="C126" s="12" t="s">
+      <c r="E128" s="18" t="s">
         <v>479</v>
       </c>
-      <c r="D126" s="16" t="s">
+      <c r="F128" s="19" t="s">
+        <v>478</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I128" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="E126" s="18" t="s">
+    </row>
+    <row r="129" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A129" s="19" t="s">
+        <v>497</v>
+      </c>
+      <c r="B129" s="19" t="s">
         <v>481</v>
       </c>
-      <c r="F126" s="19" t="s">
-        <v>480</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="H126" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I126" s="1" t="s">
+      <c r="C129" s="21" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A127" s="19" t="s">
-        <v>499</v>
-      </c>
-      <c r="B127" s="19" t="s">
+      <c r="D129" s="16" t="s">
         <v>483</v>
       </c>
-      <c r="C127" s="21" t="s">
+      <c r="E129" s="18" t="s">
         <v>484</v>
       </c>
-      <c r="D127" s="16" t="s">
+      <c r="F129" s="18" t="s">
         <v>485</v>
       </c>
-      <c r="E127" s="18" t="s">
-        <v>486</v>
-      </c>
-      <c r="F127" s="18" t="s">
-        <v>487</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H127" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" ht="93" x14ac:dyDescent="0.35">
-      <c r="A128" s="19" t="s">
-        <v>488</v>
-      </c>
-      <c r="B128" s="17" t="s">
-        <v>489</v>
-      </c>
-      <c r="C128" s="12" t="s">
-        <v>490</v>
-      </c>
-      <c r="D128" s="16" t="s">
-        <v>491</v>
-      </c>
-      <c r="E128" s="19"/>
-      <c r="F128" s="16" t="s">
-        <v>492</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H128" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I128" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A129" s="3" t="s">
-        <v>494</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="C129" s="12" t="s">
-        <v>496</v>
-      </c>
-      <c r="D129" s="21" t="s">
-        <v>497</v>
-      </c>
-      <c r="E129" s="19"/>
-      <c r="F129"/>
       <c r="G129" s="1" t="s">
         <v>62</v>
       </c>
       <c r="H129" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I129" s="1" t="s">
-        <v>498</v>
+    </row>
+    <row r="130" spans="1:9" ht="93" x14ac:dyDescent="0.35">
+      <c r="A130" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="B130" s="17" t="s">
+        <v>487</v>
+      </c>
+      <c r="C130" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="E130" s="19"/>
+      <c r="F130" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I130" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A131" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="C131" s="12" t="s">
+        <v>494</v>
+      </c>
+      <c r="D131" s="21" t="s">
+        <v>495</v>
+      </c>
+      <c r="E131" s="19"/>
+      <c r="F131"/>
+      <c r="G131" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H131" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>496</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I98">
-    <sortCondition ref="G2:G98"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I100">
+    <sortCondition ref="G4:G100"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1" xr:uid="{56461029-F272-40B0-AA7C-85F66C5CF6EB}"/>
-    <hyperlink ref="F56" r:id="rId2" xr:uid="{94D7D8F8-44B5-447E-9A32-9F64E5CCF3FA}"/>
-    <hyperlink ref="C78" r:id="rId3" xr:uid="{777A5BAE-8D61-4AA7-9259-E54BD1FDBE70}"/>
-    <hyperlink ref="C81" r:id="rId4" xr:uid="{FD026EBB-4302-4206-B780-7E1F91763261}"/>
-    <hyperlink ref="C65" r:id="rId5" xr:uid="{8966019B-4C3B-4F02-A071-5411CA74F3F8}"/>
-    <hyperlink ref="D82" r:id="rId6" xr:uid="{F64C67D3-CAF8-47D7-9BBD-60BA8702A9B2}"/>
-    <hyperlink ref="D2" r:id="rId7" xr:uid="{5E75608C-EF4E-4E89-BFD2-9C98C2096B20}"/>
-    <hyperlink ref="D4" r:id="rId8" xr:uid="{5E90B8DC-AD77-4B67-993E-32CF4C9CFD26}"/>
-    <hyperlink ref="D46" r:id="rId9" xr:uid="{097C0E3E-0A06-4C08-8729-6EE0824D62F8}"/>
-    <hyperlink ref="D96" r:id="rId10" xr:uid="{6FC1A61E-CA39-4E3B-A451-51C002A830C8}"/>
-    <hyperlink ref="D93" r:id="rId11" xr:uid="{AF63B350-6BD5-4890-B968-9E23CBF2D9C4}"/>
-    <hyperlink ref="D85" r:id="rId12" xr:uid="{68410040-0123-49F9-AD96-D8FBAF000148}"/>
-    <hyperlink ref="D49" r:id="rId13" location="programs " xr:uid="{9E90FFD4-3789-45CA-8EE0-D02F471C3648}"/>
-    <hyperlink ref="D50" r:id="rId14" xr:uid="{5DADD7F9-891C-4DA9-8630-2E4F57BA4BB0}"/>
-    <hyperlink ref="D74" r:id="rId15" xr:uid="{E7FCC05F-E0C4-4B4B-9BF6-3D5388C2BBD3}"/>
-    <hyperlink ref="D58" r:id="rId16" xr:uid="{BA7221EF-B2F7-48AC-BA37-4D01E6B77745}"/>
-    <hyperlink ref="D23" r:id="rId17" xr:uid="{94B72A5A-DA9F-4A49-B6D6-869D1EB3A773}"/>
-    <hyperlink ref="D57" r:id="rId18" xr:uid="{D1114FE8-20D3-4F80-B444-5686CFBB7223}"/>
-    <hyperlink ref="D56" r:id="rId19" xr:uid="{4A5896AC-FF3D-4F52-9EEA-57FA7C298A0F}"/>
-    <hyperlink ref="D55" r:id="rId20" xr:uid="{EB5F5F74-D4A1-4286-B2C3-3B240C8A0B3A}"/>
-    <hyperlink ref="D54" r:id="rId21" xr:uid="{A4E9F103-D8DF-4A08-B73B-82C9402281E0}"/>
-    <hyperlink ref="D51" r:id="rId22" xr:uid="{7C9B8008-6FC3-4D8B-9FAC-859864B3CCA6}"/>
-    <hyperlink ref="D59" r:id="rId23" xr:uid="{8B92366E-1104-40D7-B41A-5F9D960F675C}"/>
-    <hyperlink ref="D60" r:id="rId24" xr:uid="{BA61B788-1EE1-4D0A-BE68-5496335960B2}"/>
-    <hyperlink ref="D61" r:id="rId25" xr:uid="{788ED0D2-F799-42C7-BE70-26DAA5615100}"/>
-    <hyperlink ref="D62" r:id="rId26" xr:uid="{5315C9E9-D76A-423C-BFE1-AF451A0BCC1E}"/>
-    <hyperlink ref="D63" r:id="rId27" xr:uid="{BC82856E-908A-45D9-A41B-408B8FC5E720}"/>
-    <hyperlink ref="D64" r:id="rId28" xr:uid="{BFEA5820-6FEF-4AB5-AFDC-035AB404A7DA}"/>
-    <hyperlink ref="D65" r:id="rId29" xr:uid="{76669F61-A905-4387-B0E8-34E4D1366C7B}"/>
-    <hyperlink ref="D66" r:id="rId30" xr:uid="{74F9C236-EE46-491C-BF5A-2DFA889F7A26}"/>
-    <hyperlink ref="D67" r:id="rId31" xr:uid="{C8AC3248-2D61-4C9F-9CC4-96E24312EBEA}"/>
-    <hyperlink ref="D68" r:id="rId32" xr:uid="{B26C8AAE-4B11-4F8E-B74E-F7458BF05D09}"/>
-    <hyperlink ref="D69" r:id="rId33" xr:uid="{2A1A49A2-F37D-4774-AE8D-F594F26111D7}"/>
-    <hyperlink ref="D70" r:id="rId34" xr:uid="{9B7A9104-CDE8-4FC8-A2F3-845B8C3DB23E}"/>
-    <hyperlink ref="D71" r:id="rId35" xr:uid="{CF5BDF24-B56F-4FFF-B0DB-92F7D035BE83}"/>
-    <hyperlink ref="D72" r:id="rId36" xr:uid="{42118767-4820-49B5-A394-949C14367612}"/>
-    <hyperlink ref="D73" r:id="rId37" xr:uid="{B2C0A57F-0293-4754-8D4A-7C784AF7C213}"/>
-    <hyperlink ref="D75" r:id="rId38" xr:uid="{D07F3365-A219-44A8-BDED-0A41BC7D7571}"/>
-    <hyperlink ref="D41" r:id="rId39" xr:uid="{019C03B9-1170-401E-B03B-C29FC6CF108A}"/>
-    <hyperlink ref="C41" r:id="rId40" xr:uid="{33BA4AA8-12EB-4D42-B2D2-FB4088026AE5}"/>
-    <hyperlink ref="C16" r:id="rId41" xr:uid="{05C5E1C3-5F61-4D07-9629-20A9D90C9635}"/>
-    <hyperlink ref="C93" r:id="rId42" xr:uid="{FDB1E1E6-ADD8-4564-8753-565B078034C8}"/>
-    <hyperlink ref="D87" r:id="rId43" xr:uid="{D469BF19-F67A-4157-A0FF-1AA4B9E0BF23}"/>
-    <hyperlink ref="D35" r:id="rId44" xr:uid="{D2E0A897-D81C-4125-9C47-3A8C879089DB}"/>
-    <hyperlink ref="C35" r:id="rId45" xr:uid="{B62AA879-0896-4DFB-BBCE-B7490B146B3E}"/>
-    <hyperlink ref="C87" r:id="rId46" xr:uid="{9F59640A-1CEF-4A8B-B161-21254F4837CD}"/>
-    <hyperlink ref="D92" r:id="rId47" xr:uid="{863F960F-332F-4E54-B6FE-24604DF43AE0}"/>
-    <hyperlink ref="D47" r:id="rId48" xr:uid="{1625DFE4-6C48-4A82-8811-F4EEB64C2D2F}"/>
-    <hyperlink ref="C47" r:id="rId49" xr:uid="{7C99B3A7-0A0D-4CE1-93C6-1839F51BF301}"/>
-    <hyperlink ref="C92" r:id="rId50" xr:uid="{450BC70E-87BA-43CB-B09E-27FB7290B23E}"/>
-    <hyperlink ref="D52" r:id="rId51" xr:uid="{968FB6ED-3EE3-4000-9ED4-DED4170844E0}"/>
-    <hyperlink ref="D53" r:id="rId52" xr:uid="{F95FFAFA-D649-4148-ACBF-893459976BA3}"/>
-    <hyperlink ref="D28" r:id="rId53" xr:uid="{867A5CA1-DED0-4BC8-AA9D-0AC38C76154A}"/>
-    <hyperlink ref="C28" r:id="rId54" xr:uid="{33C23722-2292-452E-A86A-F2FF5F22AC03}"/>
-    <hyperlink ref="C17" r:id="rId55" xr:uid="{F89D664A-980E-4238-B48D-9E9A504E1383}"/>
-    <hyperlink ref="C104" r:id="rId56" xr:uid="{51C929CE-DB05-4DB6-84D8-85DAEC31CA86}"/>
-    <hyperlink ref="C105" r:id="rId57" xr:uid="{9F47A25C-362F-482B-B273-28CEF5F32C42}"/>
-    <hyperlink ref="C106" r:id="rId58" xr:uid="{64711161-99CC-43DD-9210-5E37A90E2DC5}"/>
-    <hyperlink ref="C107" r:id="rId59" xr:uid="{DF29EEE0-9F8D-4CF7-A923-7DC294F875C1}"/>
-    <hyperlink ref="C108" r:id="rId60" xr:uid="{81445D97-055E-4976-A30D-35BCE81CA70D}"/>
-    <hyperlink ref="D110" r:id="rId61" xr:uid="{693DB290-21F0-4514-9B8B-A8622C7B663B}"/>
-    <hyperlink ref="C112" r:id="rId62" xr:uid="{D55A67DC-BCF5-42B3-A86F-2339F8569063}"/>
-    <hyperlink ref="F112" r:id="rId63" display="mailto:career@albany.edu" xr:uid="{3D51B50C-49E6-4748-8F93-05F06C5C84BC}"/>
-    <hyperlink ref="C119" r:id="rId64" xr:uid="{FCB186DB-E4AB-43E4-9D1F-D223B2641022}"/>
-    <hyperlink ref="D123" r:id="rId65" xr:uid="{480FDF2F-7B59-4251-810C-73628BB15F67}"/>
-    <hyperlink ref="D125" r:id="rId66" xr:uid="{782AF740-7E61-4A73-AC61-FACCA8448159}"/>
-    <hyperlink ref="D129" r:id="rId67" xr:uid="{E8D15C86-B9A2-49FC-8FBA-DD6355B5091B}"/>
-    <hyperlink ref="C126" r:id="rId68" xr:uid="{604F38FE-1039-4EE3-8E74-8165B8FF8430}"/>
-    <hyperlink ref="C127" r:id="rId69" xr:uid="{F0014F07-00B7-439A-9BE1-6BAE3ECD85AC}"/>
-    <hyperlink ref="C128" r:id="rId70" xr:uid="{82004575-EEEF-4DDF-972C-9340A1AA43F5}"/>
-    <hyperlink ref="C125" r:id="rId71" xr:uid="{74182992-2721-4728-8FE1-43CF72383D38}"/>
-    <hyperlink ref="C129" r:id="rId72" xr:uid="{7EBFD176-16F3-4D24-9E15-870D3D96750B}"/>
+    <hyperlink ref="F25" r:id="rId1" xr:uid="{56461029-F272-40B0-AA7C-85F66C5CF6EB}"/>
+    <hyperlink ref="F58" r:id="rId2" xr:uid="{94D7D8F8-44B5-447E-9A32-9F64E5CCF3FA}"/>
+    <hyperlink ref="C80" r:id="rId3" xr:uid="{777A5BAE-8D61-4AA7-9259-E54BD1FDBE70}"/>
+    <hyperlink ref="C83" r:id="rId4" xr:uid="{FD026EBB-4302-4206-B780-7E1F91763261}"/>
+    <hyperlink ref="C67" r:id="rId5" xr:uid="{8966019B-4C3B-4F02-A071-5411CA74F3F8}"/>
+    <hyperlink ref="D84" r:id="rId6" xr:uid="{F64C67D3-CAF8-47D7-9BBD-60BA8702A9B2}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{5E75608C-EF4E-4E89-BFD2-9C98C2096B20}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{5E90B8DC-AD77-4B67-993E-32CF4C9CFD26}"/>
+    <hyperlink ref="D48" r:id="rId9" xr:uid="{097C0E3E-0A06-4C08-8729-6EE0824D62F8}"/>
+    <hyperlink ref="D98" r:id="rId10" xr:uid="{6FC1A61E-CA39-4E3B-A451-51C002A830C8}"/>
+    <hyperlink ref="D95" r:id="rId11" xr:uid="{AF63B350-6BD5-4890-B968-9E23CBF2D9C4}"/>
+    <hyperlink ref="D87" r:id="rId12" xr:uid="{68410040-0123-49F9-AD96-D8FBAF000148}"/>
+    <hyperlink ref="D51" r:id="rId13" location="programs " xr:uid="{9E90FFD4-3789-45CA-8EE0-D02F471C3648}"/>
+    <hyperlink ref="D52" r:id="rId14" xr:uid="{5DADD7F9-891C-4DA9-8630-2E4F57BA4BB0}"/>
+    <hyperlink ref="D76" r:id="rId15" xr:uid="{E7FCC05F-E0C4-4B4B-9BF6-3D5388C2BBD3}"/>
+    <hyperlink ref="D60" r:id="rId16" xr:uid="{BA7221EF-B2F7-48AC-BA37-4D01E6B77745}"/>
+    <hyperlink ref="D25" r:id="rId17" xr:uid="{94B72A5A-DA9F-4A49-B6D6-869D1EB3A773}"/>
+    <hyperlink ref="D59" r:id="rId18" xr:uid="{D1114FE8-20D3-4F80-B444-5686CFBB7223}"/>
+    <hyperlink ref="D58" r:id="rId19" xr:uid="{4A5896AC-FF3D-4F52-9EEA-57FA7C298A0F}"/>
+    <hyperlink ref="D57" r:id="rId20" xr:uid="{EB5F5F74-D4A1-4286-B2C3-3B240C8A0B3A}"/>
+    <hyperlink ref="D56" r:id="rId21" xr:uid="{A4E9F103-D8DF-4A08-B73B-82C9402281E0}"/>
+    <hyperlink ref="D53" r:id="rId22" xr:uid="{7C9B8008-6FC3-4D8B-9FAC-859864B3CCA6}"/>
+    <hyperlink ref="D61" r:id="rId23" xr:uid="{8B92366E-1104-40D7-B41A-5F9D960F675C}"/>
+    <hyperlink ref="D62" r:id="rId24" xr:uid="{BA61B788-1EE1-4D0A-BE68-5496335960B2}"/>
+    <hyperlink ref="D63" r:id="rId25" xr:uid="{788ED0D2-F799-42C7-BE70-26DAA5615100}"/>
+    <hyperlink ref="D64" r:id="rId26" xr:uid="{5315C9E9-D76A-423C-BFE1-AF451A0BCC1E}"/>
+    <hyperlink ref="D65" r:id="rId27" xr:uid="{BC82856E-908A-45D9-A41B-408B8FC5E720}"/>
+    <hyperlink ref="D66" r:id="rId28" xr:uid="{BFEA5820-6FEF-4AB5-AFDC-035AB404A7DA}"/>
+    <hyperlink ref="D67" r:id="rId29" xr:uid="{76669F61-A905-4387-B0E8-34E4D1366C7B}"/>
+    <hyperlink ref="D68" r:id="rId30" xr:uid="{74F9C236-EE46-491C-BF5A-2DFA889F7A26}"/>
+    <hyperlink ref="D69" r:id="rId31" xr:uid="{C8AC3248-2D61-4C9F-9CC4-96E24312EBEA}"/>
+    <hyperlink ref="D70" r:id="rId32" xr:uid="{B26C8AAE-4B11-4F8E-B74E-F7458BF05D09}"/>
+    <hyperlink ref="D71" r:id="rId33" xr:uid="{2A1A49A2-F37D-4774-AE8D-F594F26111D7}"/>
+    <hyperlink ref="D72" r:id="rId34" xr:uid="{9B7A9104-CDE8-4FC8-A2F3-845B8C3DB23E}"/>
+    <hyperlink ref="D73" r:id="rId35" xr:uid="{CF5BDF24-B56F-4FFF-B0DB-92F7D035BE83}"/>
+    <hyperlink ref="D74" r:id="rId36" xr:uid="{42118767-4820-49B5-A394-949C14367612}"/>
+    <hyperlink ref="D75" r:id="rId37" xr:uid="{B2C0A57F-0293-4754-8D4A-7C784AF7C213}"/>
+    <hyperlink ref="D77" r:id="rId38" xr:uid="{D07F3365-A219-44A8-BDED-0A41BC7D7571}"/>
+    <hyperlink ref="D43" r:id="rId39" xr:uid="{019C03B9-1170-401E-B03B-C29FC6CF108A}"/>
+    <hyperlink ref="C43" r:id="rId40" xr:uid="{33BA4AA8-12EB-4D42-B2D2-FB4088026AE5}"/>
+    <hyperlink ref="C18" r:id="rId41" xr:uid="{05C5E1C3-5F61-4D07-9629-20A9D90C9635}"/>
+    <hyperlink ref="C95" r:id="rId42" xr:uid="{FDB1E1E6-ADD8-4564-8753-565B078034C8}"/>
+    <hyperlink ref="D89" r:id="rId43" xr:uid="{D469BF19-F67A-4157-A0FF-1AA4B9E0BF23}"/>
+    <hyperlink ref="D37" r:id="rId44" xr:uid="{D2E0A897-D81C-4125-9C47-3A8C879089DB}"/>
+    <hyperlink ref="C37" r:id="rId45" xr:uid="{B62AA879-0896-4DFB-BBCE-B7490B146B3E}"/>
+    <hyperlink ref="C89" r:id="rId46" xr:uid="{9F59640A-1CEF-4A8B-B161-21254F4837CD}"/>
+    <hyperlink ref="D94" r:id="rId47" xr:uid="{863F960F-332F-4E54-B6FE-24604DF43AE0}"/>
+    <hyperlink ref="D49" r:id="rId48" xr:uid="{1625DFE4-6C48-4A82-8811-F4EEB64C2D2F}"/>
+    <hyperlink ref="C49" r:id="rId49" xr:uid="{7C99B3A7-0A0D-4CE1-93C6-1839F51BF301}"/>
+    <hyperlink ref="C94" r:id="rId50" xr:uid="{450BC70E-87BA-43CB-B09E-27FB7290B23E}"/>
+    <hyperlink ref="D54" r:id="rId51" xr:uid="{968FB6ED-3EE3-4000-9ED4-DED4170844E0}"/>
+    <hyperlink ref="D55" r:id="rId52" xr:uid="{F95FFAFA-D649-4148-ACBF-893459976BA3}"/>
+    <hyperlink ref="D30" r:id="rId53" xr:uid="{867A5CA1-DED0-4BC8-AA9D-0AC38C76154A}"/>
+    <hyperlink ref="C30" r:id="rId54" xr:uid="{33C23722-2292-452E-A86A-F2FF5F22AC03}"/>
+    <hyperlink ref="C19" r:id="rId55" xr:uid="{F89D664A-980E-4238-B48D-9E9A504E1383}"/>
+    <hyperlink ref="C106" r:id="rId56" xr:uid="{51C929CE-DB05-4DB6-84D8-85DAEC31CA86}"/>
+    <hyperlink ref="C107" r:id="rId57" xr:uid="{9F47A25C-362F-482B-B273-28CEF5F32C42}"/>
+    <hyperlink ref="C108" r:id="rId58" xr:uid="{64711161-99CC-43DD-9210-5E37A90E2DC5}"/>
+    <hyperlink ref="C109" r:id="rId59" xr:uid="{DF29EEE0-9F8D-4CF7-A923-7DC294F875C1}"/>
+    <hyperlink ref="C110" r:id="rId60" xr:uid="{81445D97-055E-4976-A30D-35BCE81CA70D}"/>
+    <hyperlink ref="D112" r:id="rId61" xr:uid="{693DB290-21F0-4514-9B8B-A8622C7B663B}"/>
+    <hyperlink ref="C114" r:id="rId62" xr:uid="{D55A67DC-BCF5-42B3-A86F-2339F8569063}"/>
+    <hyperlink ref="F114" r:id="rId63" display="mailto:career@albany.edu" xr:uid="{3D51B50C-49E6-4748-8F93-05F06C5C84BC}"/>
+    <hyperlink ref="C121" r:id="rId64" xr:uid="{FCB186DB-E4AB-43E4-9D1F-D223B2641022}"/>
+    <hyperlink ref="D125" r:id="rId65" xr:uid="{480FDF2F-7B59-4251-810C-73628BB15F67}"/>
+    <hyperlink ref="D127" r:id="rId66" xr:uid="{782AF740-7E61-4A73-AC61-FACCA8448159}"/>
+    <hyperlink ref="D131" r:id="rId67" xr:uid="{E8D15C86-B9A2-49FC-8FBA-DD6355B5091B}"/>
+    <hyperlink ref="C128" r:id="rId68" xr:uid="{604F38FE-1039-4EE3-8E74-8165B8FF8430}"/>
+    <hyperlink ref="C129" r:id="rId69" xr:uid="{F0014F07-00B7-439A-9BE1-6BAE3ECD85AC}"/>
+    <hyperlink ref="C130" r:id="rId70" xr:uid="{82004575-EEEF-4DDF-972C-9340A1AA43F5}"/>
+    <hyperlink ref="C127" r:id="rId71" xr:uid="{74182992-2721-4728-8FE1-43CF72383D38}"/>
+    <hyperlink ref="C131" r:id="rId72" xr:uid="{7EBFD176-16F3-4D24-9E15-870D3D96750B}"/>
+    <hyperlink ref="F2" r:id="rId73" xr:uid="{0F9AD5BE-0C46-4CBA-ABED-01801389D4B4}"/>
+    <hyperlink ref="C2" r:id="rId74" xr:uid="{7488EE3C-4876-41B7-AD1C-E59148EF5C60}"/>
+    <hyperlink ref="F3" r:id="rId75" xr:uid="{94D425E2-BDB7-40FE-AC8D-A0E405381B9B}"/>
+    <hyperlink ref="C3" r:id="rId76" xr:uid="{8771AA61-5955-4023-916F-EA0D148D2A7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId73"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId77"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed Middle Earth Address
</commit_message>
<xml_diff>
--- a/data-raw/Rolodex.xlsx
+++ b/data-raw/Rolodex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\OneDrive\Desktop\New Shiny Apps\Rolodex\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FE2997-9D8B-4445-BFA7-A352A24EFC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1772AAE1-CD30-454F-AD19-76C5D117A790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="0" windowWidth="19200" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rolodex NEW" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="504">
   <si>
     <t>Name</t>
   </si>
@@ -486,9 +486,6 @@
   </si>
   <si>
     <t>Health and Counseling Services Building (ground level of Dutch Quad)</t>
-  </si>
-  <si>
-    <t>Seneca Hall B005, Indigenous Quad</t>
   </si>
   <si>
     <t>Campus Center 137</t>
@@ -2559,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2605,20 +2602,20 @@
     </row>
     <row r="2" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="22" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>105</v>
@@ -2627,25 +2624,25 @@
         <v>10</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="22" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>96</v>
@@ -2654,25 +2651,25 @@
         <v>10</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="22" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>52</v>
@@ -2681,25 +2678,25 @@
         <v>10</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="22" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>79</v>
@@ -2708,25 +2705,25 @@
         <v>10</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="22" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>86</v>
@@ -2735,7 +2732,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -2746,13 +2743,13 @@
         <v>142</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>133</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>134</v>
@@ -2764,7 +2761,7 @@
         <v>26</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
@@ -2772,16 +2769,16 @@
         <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>31</v>
@@ -2793,7 +2790,7 @@
         <v>26</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -2804,13 +2801,13 @@
         <v>143</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>35</v>
@@ -2822,7 +2819,7 @@
         <v>26</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2830,16 +2827,16 @@
         <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>38</v>
@@ -2851,7 +2848,7 @@
         <v>26</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -2862,7 +2859,7 @@
         <v>144</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>40</v>
@@ -2878,7 +2875,7 @@
         <v>26</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -2889,7 +2886,7 @@
         <v>144</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>43</v>
@@ -2905,7 +2902,7 @@
         <v>26</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -2916,7 +2913,7 @@
         <v>144</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>46</v>
@@ -2932,7 +2929,7 @@
         <v>26</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -2943,13 +2940,13 @@
         <v>145</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>50</v>
@@ -2961,16 +2958,16 @@
         <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>51</v>
@@ -2984,15 +2981,15 @@
         <v>10</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>51</v>
@@ -3004,16 +3001,16 @@
         <v>10</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>52</v>
@@ -3022,16 +3019,16 @@
         <v>10</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>52</v>
@@ -3040,7 +3037,7 @@
         <v>10</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -3049,7 +3046,7 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>54</v>
@@ -3065,7 +3062,7 @@
         <v>26</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -3073,13 +3070,13 @@
         <v>85</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -3090,7 +3087,7 @@
         <v>10</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -3098,10 +3095,10 @@
         <v>136</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>88</v>
@@ -3115,18 +3112,18 @@
         <v>10</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>338</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>339</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>52</v>
@@ -3135,7 +3132,7 @@
         <v>10</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -3146,13 +3143,13 @@
         <v>144</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>58</v>
@@ -3164,7 +3161,7 @@
         <v>26</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -3175,13 +3172,13 @@
         <v>144</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>58</v>
@@ -3193,7 +3190,7 @@
         <v>26</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -3204,13 +3201,13 @@
         <v>144</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>58</v>
@@ -3222,7 +3219,7 @@
         <v>26</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -3233,13 +3230,13 @@
         <v>144</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>58</v>
@@ -3251,7 +3248,7 @@
         <v>26</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -3262,13 +3259,13 @@
         <v>144</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>58</v>
@@ -3280,7 +3277,7 @@
         <v>26</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -3291,16 +3288,16 @@
         <v>146</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>194</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>62</v>
@@ -3309,7 +3306,7 @@
         <v>26</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -3320,13 +3317,13 @@
         <v>147</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>50</v>
@@ -3338,7 +3335,7 @@
         <v>26</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -3349,7 +3346,7 @@
         <v>148</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>65</v>
@@ -3358,7 +3355,7 @@
         <v>64</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>62</v>
@@ -3367,7 +3364,7 @@
         <v>26</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -3378,7 +3375,7 @@
         <v>149</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>67</v>
@@ -3394,27 +3391,27 @@
         <v>26</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="G32" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -3423,95 +3420,95 @@
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="G34" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="G35" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>357</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="G36" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>360</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="G37" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -3519,13 +3516,13 @@
         <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>70</v>
@@ -3538,7 +3535,7 @@
         <v>10</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="31" x14ac:dyDescent="0.35">
@@ -3546,16 +3543,16 @@
         <v>14</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>16</v>
@@ -3567,7 +3564,7 @@
         <v>10</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -3575,13 +3572,13 @@
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
@@ -3594,7 +3591,7 @@
         <v>10</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -3602,13 +3599,13 @@
         <v>19</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -3619,21 +3616,21 @@
         <v>10</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>72</v>
@@ -3648,7 +3645,7 @@
         <v>10</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -3656,16 +3653,16 @@
         <v>8</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
@@ -3675,7 +3672,7 @@
         <v>10</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -3686,13 +3683,13 @@
         <v>150</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>77</v>
@@ -3704,7 +3701,7 @@
         <v>26</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -3713,10 +3710,10 @@
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -3727,7 +3724,7 @@
         <v>10</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -3736,10 +3733,10 @@
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -3750,7 +3747,7 @@
         <v>10</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -3759,10 +3756,10 @@
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -3773,7 +3770,7 @@
         <v>10</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -3782,13 +3779,13 @@
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
@@ -3798,16 +3795,16 @@
         <v>10</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>83</v>
@@ -3821,18 +3818,18 @@
         <v>10</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>353</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>354</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>79</v>
@@ -3841,7 +3838,7 @@
         <v>10</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
@@ -3849,10 +3846,10 @@
         <v>141</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>329</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>28</v>
@@ -3866,7 +3863,7 @@
         <v>26</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
@@ -3874,13 +3871,13 @@
         <v>27</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -3891,7 +3888,7 @@
         <v>10</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -3899,16 +3896,16 @@
         <v>8</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
@@ -3918,7 +3915,7 @@
         <v>10</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -3927,14 +3924,14 @@
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>87</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>86</v>
@@ -3943,7 +3940,7 @@
         <v>10</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -3954,13 +3951,13 @@
         <v>150</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>90</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>91</v>
@@ -3972,24 +3969,22 @@
         <v>26</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>151</v>
-      </c>
+      <c r="B56" s="1"/>
       <c r="C56" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>93</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>94</v>
@@ -4001,15 +3996,15 @@
         <v>26</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>344</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>86</v>
@@ -4018,15 +4013,15 @@
         <v>10</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>86</v>
@@ -4035,7 +4030,7 @@
         <v>10</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -4044,10 +4039,10 @@
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -4058,7 +4053,7 @@
         <v>10</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
@@ -4067,10 +4062,10 @@
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -4081,7 +4076,7 @@
         <v>10</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
@@ -4090,14 +4085,14 @@
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>99</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>96</v>
@@ -4106,19 +4101,19 @@
         <v>10</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -4129,7 +4124,7 @@
         <v>10</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -4138,10 +4133,10 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -4152,7 +4147,7 @@
         <v>10</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -4161,10 +4156,10 @@
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -4175,7 +4170,7 @@
         <v>10</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -4184,10 +4179,10 @@
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -4198,7 +4193,7 @@
         <v>10</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -4207,10 +4202,10 @@
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -4221,7 +4216,7 @@
         <v>10</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -4230,10 +4225,10 @@
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -4244,7 +4239,7 @@
         <v>10</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -4253,10 +4248,10 @@
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -4267,7 +4262,7 @@
         <v>10</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -4276,10 +4271,10 @@
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -4290,7 +4285,7 @@
         <v>10</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -4298,13 +4293,13 @@
         <v>114</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -4315,7 +4310,7 @@
         <v>10</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -4324,10 +4319,10 @@
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -4338,7 +4333,7 @@
         <v>10</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
@@ -4347,7 +4342,7 @@
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>107</v>
@@ -4361,7 +4356,7 @@
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -4370,10 +4365,10 @@
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -4384,7 +4379,7 @@
         <v>10</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -4393,10 +4388,10 @@
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -4407,7 +4402,7 @@
         <v>10</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -4416,7 +4411,7 @@
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>111</v>
@@ -4430,7 +4425,7 @@
         <v>10</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
@@ -4439,7 +4434,7 @@
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>113</v>
@@ -4453,7 +4448,7 @@
         <v>10</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -4462,10 +4457,10 @@
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -4476,7 +4471,7 @@
         <v>10</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
@@ -4485,10 +4480,10 @@
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -4499,7 +4494,7 @@
         <v>10</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
@@ -4507,16 +4502,16 @@
         <v>11</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>13</v>
@@ -4528,7 +4523,7 @@
         <v>10</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
@@ -4536,13 +4531,13 @@
         <v>116</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
@@ -4555,7 +4550,7 @@
         <v>10</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
@@ -4563,13 +4558,13 @@
         <v>118</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -4580,21 +4575,21 @@
         <v>10</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C82" s="3" t="s">
+      <c r="D82" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -4605,7 +4600,7 @@
         <v>10</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -4613,16 +4608,16 @@
         <v>119</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C83" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="D83" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
@@ -4632,7 +4627,7 @@
         <v>10</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -4640,13 +4635,13 @@
         <v>120</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
@@ -4657,7 +4652,7 @@
         <v>10</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
@@ -4665,13 +4660,13 @@
         <v>121</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -4682,7 +4677,7 @@
         <v>10</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
@@ -4693,13 +4688,13 @@
         <v>150</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>77</v>
@@ -4711,7 +4706,7 @@
         <v>26</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -4719,10 +4714,10 @@
         <v>122</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>124</v>
@@ -4740,7 +4735,7 @@
         <v>26</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
@@ -4751,13 +4746,13 @@
         <v>150</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D88" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E88" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>25</v>
@@ -4769,7 +4764,7 @@
         <v>26</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -4777,16 +4772,16 @@
         <v>8</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
@@ -4796,7 +4791,7 @@
         <v>10</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -4804,16 +4799,16 @@
         <v>11</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>13</v>
@@ -4825,7 +4820,7 @@
         <v>10</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="31" x14ac:dyDescent="0.35">
@@ -4833,16 +4828,16 @@
         <v>14</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>16</v>
@@ -4854,7 +4849,7 @@
         <v>10</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
@@ -4862,13 +4857,13 @@
         <v>17</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
@@ -4881,7 +4876,7 @@
         <v>10</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
@@ -4889,13 +4884,13 @@
         <v>19</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -4906,7 +4901,7 @@
         <v>10</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
@@ -4915,7 +4910,7 @@
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>21</v>
@@ -4929,7 +4924,7 @@
         <v>10</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
@@ -4938,7 +4933,7 @@
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>23</v>
@@ -4952,7 +4947,7 @@
         <v>10</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -4963,13 +4958,13 @@
         <v>150</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D96" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>25</v>
@@ -4981,7 +4976,7 @@
         <v>26</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -4989,13 +4984,13 @@
         <v>27</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -5006,7 +5001,7 @@
         <v>10</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
@@ -5014,10 +5009,10 @@
         <v>141</v>
       </c>
       <c r="B98" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C98" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>329</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>28</v>
@@ -5031,7 +5026,7 @@
         <v>26</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
@@ -5040,10 +5035,10 @@
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
@@ -5054,21 +5049,21 @@
         <v>10</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
@@ -5081,7 +5076,7 @@
         <v>26</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
@@ -5089,10 +5084,10 @@
         <v>141</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>328</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>329</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>28</v>
@@ -5106,16 +5101,16 @@
         <v>26</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>83</v>
@@ -5129,18 +5124,18 @@
         <v>10</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>128</v>
@@ -5156,15 +5151,15 @@
         <v>10</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>367</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>368</v>
       </c>
       <c r="G104" s="3" t="s">
         <v>79</v>
@@ -5173,15 +5168,15 @@
         <v>10</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D105" s="3" t="s">
         <v>370</v>
-      </c>
-      <c r="D105" s="3" t="s">
-        <v>371</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>52</v>
@@ -5190,15 +5185,15 @@
         <v>10</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>52</v>
@@ -5207,15 +5202,15 @@
         <v>10</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>52</v>
@@ -5224,15 +5219,15 @@
         <v>10</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>52</v>
@@ -5241,21 +5236,21 @@
         <v>10</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C109" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="C109" s="12" t="s">
+      <c r="D109" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D109" s="3" t="s">
-        <v>393</v>
-      </c>
       <c r="E109" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>86</v>
@@ -5264,21 +5259,21 @@
         <v>10</v>
       </c>
       <c r="I109" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C110" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="C110" s="12" t="s">
+      <c r="D110" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D110" s="3" t="s">
-        <v>393</v>
-      </c>
       <c r="E110" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>79</v>
@@ -5287,21 +5282,21 @@
         <v>10</v>
       </c>
       <c r="I110" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C111" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="C111" s="12" t="s">
+      <c r="D111" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D111" s="3" t="s">
-        <v>393</v>
-      </c>
       <c r="E111" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>96</v>
@@ -5310,21 +5305,21 @@
         <v>10</v>
       </c>
       <c r="I111" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C112" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="C112" s="12" t="s">
+      <c r="D112" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D112" s="3" t="s">
-        <v>393</v>
-      </c>
       <c r="E112" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>105</v>
@@ -5333,21 +5328,21 @@
         <v>10</v>
       </c>
       <c r="I112" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C113" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="C113" s="12" t="s">
+      <c r="D113" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>393</v>
-      </c>
       <c r="E113" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>9</v>
@@ -5356,21 +5351,21 @@
         <v>10</v>
       </c>
       <c r="I113" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="D114" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="E114" s="3" t="s">
         <v>397</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>398</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>9</v>
@@ -5379,67 +5374,67 @@
         <v>10</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D115" s="12" t="s">
         <v>400</v>
       </c>
-      <c r="D115" s="12" t="s">
+      <c r="E115" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I115" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E116" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="G116" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="G116" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="H116" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B117" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="C117" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="C117" s="12" t="s">
+      <c r="D117" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="D117" s="3" t="s">
+      <c r="E117" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="F117" s="12" t="s">
         <v>409</v>
-      </c>
-      <c r="F117" s="12" t="s">
-        <v>410</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>32</v>
@@ -5448,7 +5443,7 @@
         <v>26</v>
       </c>
       <c r="I117" s="13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5456,96 +5451,96 @@
         <v>85</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C118" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="D118" s="14" t="s">
         <v>413</v>
       </c>
-      <c r="D118" s="14" t="s">
+      <c r="E118" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="E118" s="15" t="s">
+      <c r="F118" t="s">
         <v>415</v>
       </c>
-      <c r="F118" t="s">
+      <c r="G118" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="G118" s="14" t="s">
+      <c r="H118" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I118" s="10" t="s">
         <v>417</v>
-      </c>
-      <c r="H118" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I118" s="10" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A119" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="B119" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="B119" s="14" t="s">
+      <c r="C119" t="s">
         <v>420</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="E119" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="D119" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="E119" s="15" t="s">
+      <c r="F119" t="s">
         <v>422</v>
       </c>
-      <c r="F119" t="s">
-        <v>423</v>
-      </c>
       <c r="G119" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H119" s="14" t="s">
         <v>26</v>
       </c>
       <c r="I119" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B120" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C120" t="s">
         <v>425</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="D120" s="14" t="s">
+      <c r="E120" s="15" t="s">
         <v>427</v>
-      </c>
-      <c r="E120" s="15" t="s">
-        <v>428</v>
       </c>
       <c r="F120" t="s">
         <v>126</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H120" s="14" t="s">
         <v>10</v>
       </c>
       <c r="I120" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B121" s="12"/>
       <c r="C121" s="14"/>
       <c r="D121" s="14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E121" s="14"/>
       <c r="F121" s="14"/>
@@ -5556,27 +5551,27 @@
         <v>10</v>
       </c>
       <c r="I121" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A122" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="B122" s="14" t="s">
         <v>433</v>
       </c>
-      <c r="B122" s="14" t="s">
+      <c r="C122" t="s">
         <v>434</v>
       </c>
-      <c r="C122" t="s">
+      <c r="D122" s="14" t="s">
         <v>435</v>
       </c>
-      <c r="D122" s="14" t="s">
+      <c r="E122" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="F122" t="s">
         <v>436</v>
-      </c>
-      <c r="E122" s="14" t="s">
-        <v>447</v>
-      </c>
-      <c r="F122" t="s">
-        <v>437</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>62</v>
@@ -5585,27 +5580,27 @@
         <v>10</v>
       </c>
       <c r="I122" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A123" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="B123" s="14" t="s">
         <v>439</v>
       </c>
-      <c r="B123" s="14" t="s">
+      <c r="C123" t="s">
         <v>440</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" s="14" t="s">
         <v>441</v>
       </c>
-      <c r="D123" s="14" t="s">
+      <c r="E123" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="F123" t="s">
         <v>442</v>
-      </c>
-      <c r="E123" s="14" t="s">
-        <v>446</v>
-      </c>
-      <c r="F123" t="s">
-        <v>443</v>
       </c>
       <c r="G123" s="14" t="s">
         <v>32</v>
@@ -5614,24 +5609,24 @@
         <v>26</v>
       </c>
       <c r="I123" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="B124" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="B124" s="3" t="s">
-        <v>452</v>
-      </c>
       <c r="C124" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>84</v>
@@ -5640,21 +5635,21 @@
         <v>26</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="D125" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="E125" s="3" t="s">
         <v>455</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>456</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>52</v>
@@ -5663,21 +5658,21 @@
         <v>10</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="D126" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="E126" s="3" t="s">
         <v>455</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>456</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>79</v>
@@ -5686,18 +5681,18 @@
         <v>10</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="93" x14ac:dyDescent="0.35">
       <c r="A127" s="16" t="s">
+        <v>457</v>
+      </c>
+      <c r="B127" s="17" t="s">
         <v>458</v>
       </c>
-      <c r="B127" s="17" t="s">
+      <c r="D127" s="16" t="s">
         <v>459</v>
-      </c>
-      <c r="D127" s="16" t="s">
-        <v>460</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>115</v>
@@ -5706,21 +5701,21 @@
         <v>10</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A128" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="B128" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="D128" s="12" t="s">
         <v>463</v>
       </c>
-      <c r="D128" s="12" t="s">
+      <c r="F128" s="18" t="s">
         <v>464</v>
-      </c>
-      <c r="F128" s="18" t="s">
-        <v>465</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>115</v>
@@ -5729,18 +5724,18 @@
         <v>10</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B129" s="16" t="s">
         <v>467</v>
       </c>
-      <c r="B129" s="16" t="s">
+      <c r="F129" s="3" t="s">
         <v>468</v>
-      </c>
-      <c r="F129" s="3" t="s">
-        <v>469</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>115</v>
@@ -5749,24 +5744,24 @@
         <v>10</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B130" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C130" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="C130" s="12" t="s">
+      <c r="D130" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="D130" s="12" t="s">
+      <c r="F130" s="20" t="s">
         <v>473</v>
-      </c>
-      <c r="F130" s="20" t="s">
-        <v>474</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>115</v>
@@ -5777,22 +5772,22 @@
     </row>
     <row r="131" spans="1:9" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A131" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="B131" s="19" t="s">
         <v>475</v>
       </c>
-      <c r="B131" s="19" t="s">
+      <c r="C131" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="C131" s="12" t="s">
+      <c r="D131" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="D131" s="16" t="s">
+      <c r="E131" s="18" t="s">
         <v>478</v>
       </c>
-      <c r="E131" s="18" t="s">
-        <v>479</v>
-      </c>
       <c r="F131" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>115</v>
@@ -5801,27 +5796,27 @@
         <v>10</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A132" s="19" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B132" s="19" t="s">
+        <v>480</v>
+      </c>
+      <c r="C132" s="21" t="s">
         <v>481</v>
       </c>
-      <c r="C132" s="21" t="s">
+      <c r="D132" s="16" t="s">
         <v>482</v>
       </c>
-      <c r="D132" s="16" t="s">
+      <c r="E132" s="18" t="s">
         <v>483</v>
       </c>
-      <c r="E132" s="18" t="s">
+      <c r="F132" s="18" t="s">
         <v>484</v>
-      </c>
-      <c r="F132" s="18" t="s">
-        <v>485</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>62</v>
@@ -5832,20 +5827,20 @@
     </row>
     <row r="133" spans="1:9" ht="93" x14ac:dyDescent="0.35">
       <c r="A133" s="19" t="s">
+        <v>485</v>
+      </c>
+      <c r="B133" s="17" t="s">
         <v>486</v>
       </c>
-      <c r="B133" s="17" t="s">
+      <c r="C133" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="C133" s="12" t="s">
+      <c r="D133" s="16" t="s">
         <v>488</v>
-      </c>
-      <c r="D133" s="16" t="s">
-        <v>489</v>
       </c>
       <c r="E133" s="19"/>
       <c r="F133" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>62</v>
@@ -5854,21 +5849,21 @@
         <v>10</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B134" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="B134" s="3" t="s">
+      <c r="C134" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="C134" s="12" t="s">
+      <c r="D134" s="21" t="s">
         <v>494</v>
-      </c>
-      <c r="D134" s="21" t="s">
-        <v>495</v>
       </c>
       <c r="E134" s="19"/>
       <c r="F134"/>
@@ -5879,7 +5874,7 @@
         <v>10</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated tutoring (Undergrad only)
</commit_message>
<xml_diff>
--- a/data-raw/Rolodex.xlsx
+++ b/data-raw/Rolodex.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\New Shiny Apps\Rolodex\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF15B763-759E-47A2-B0D4-90EF2201320F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F69085-E0BD-42C1-8BFC-9E90F53EE145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,9 +143,6 @@
     <t>writing@albany.edu</t>
   </si>
   <si>
-    <t>Tutoring</t>
-  </si>
-  <si>
     <t>https://www.albany.edu/academic-advising/tutoring#additionalresources</t>
   </si>
   <si>
@@ -560,9 +557,6 @@
   </si>
   <si>
     <t>Writing, research, and teaching support</t>
-  </si>
-  <si>
-    <t>Peer tutoring - study buddies - workshops - departmental tutoring</t>
   </si>
   <si>
     <t>M-F: 8:30 AM - 5 PM</t>
@@ -1695,6 +1689,12 @@
   </si>
   <si>
     <t>tel:518-442-4900</t>
+  </si>
+  <si>
+    <t>Tutoring</t>
+  </si>
+  <si>
+    <t>Undergrads Only - Peer tutoring - study buddies - workshops - departmental tutoring</t>
   </si>
 </sst>
 </file>
@@ -2267,7 +2267,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2298,7 +2298,6 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2657,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E106" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I141" sqref="I141"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2698,162 +2697,162 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>32</v>
@@ -2862,7 +2861,7 @@
         <v>26</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -2870,16 +2869,16 @@
         <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>31</v>
@@ -2891,7 +2890,7 @@
         <v>26</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -2899,16 +2898,16 @@
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>35</v>
@@ -2920,27 +2919,27 @@
         <v>26</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>32</v>
@@ -2949,25 +2948,25 @@
         <v>26</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>175</v>
+        <v>534</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>32</v>
@@ -2976,25 +2975,25 @@
         <v>26</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>32</v>
@@ -3003,25 +3002,25 @@
         <v>26</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>32</v>
@@ -3030,27 +3029,27 @@
         <v>26</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>32</v>
@@ -3059,582 +3058,582 @@
         <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="H16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>385</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>382</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>335</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="H32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="8" t="s">
         <v>353</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="9" t="s">
         <v>356</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="G37" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -3642,28 +3641,28 @@
         <v>14</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -3671,26 +3670,26 @@
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -3698,53 +3697,53 @@
         <v>19</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="G42" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -3752,203 +3751,203 @@
         <v>8</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="G44" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>28</v>
@@ -3956,13 +3955,13 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
@@ -3970,24 +3969,24 @@
         <v>27</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -3995,235 +3994,235 @@
         <v>8</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D55" s="4" t="s">
+      <c r="E55" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="G55" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D56" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="G56" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -4232,90 +4231,90 @@
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -4324,92 +4323,92 @@
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -4418,159 +4417,159 @@
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
@@ -4579,21 +4578,21 @@
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
@@ -4601,240 +4600,240 @@
         <v>11</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>13</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H82" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H83" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="D86" s="1" t="s">
+      <c r="E86" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="G86" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E87" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="D87" s="4" t="s">
+      <c r="F87" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="G87" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
@@ -4842,28 +4841,28 @@
         <v>24</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -4871,16 +4870,16 @@
         <v>8</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
@@ -4890,7 +4889,7 @@
         <v>10</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -4898,16 +4897,16 @@
         <v>11</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>13</v>
@@ -4919,7 +4918,7 @@
         <v>10</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
@@ -4927,16 +4926,16 @@
         <v>14</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>16</v>
@@ -4948,7 +4947,7 @@
         <v>10</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
@@ -4956,13 +4955,13 @@
         <v>17</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
@@ -4975,7 +4974,7 @@
         <v>10</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
@@ -4983,13 +4982,13 @@
         <v>19</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C93" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>307</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -5000,7 +4999,7 @@
         <v>10</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
@@ -5009,7 +5008,7 @@
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>21</v>
@@ -5023,7 +5022,7 @@
         <v>10</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
@@ -5032,7 +5031,7 @@
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>23</v>
@@ -5046,7 +5045,7 @@
         <v>10</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -5054,16 +5053,16 @@
         <v>24</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>25</v>
@@ -5075,7 +5074,7 @@
         <v>26</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -5083,13 +5082,13 @@
         <v>27</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -5100,18 +5099,18 @@
         <v>10</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>28</v>
@@ -5125,68 +5124,68 @@
         <v>26</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>28</v>
@@ -5194,254 +5193,254 @@
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="G103" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="H103" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I104" s="1" t="s">
         <v>364</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H104" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I105" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H105" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I105" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H106" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H107" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G108" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H108" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D109" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C109" s="6" t="s">
+      <c r="E109" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I109" s="8" t="s">
         <v>389</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H109" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I109" s="8" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="E110" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I110" s="8" t="s">
         <v>389</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="G110" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H110" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I110" s="8" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D111" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C111" s="6" t="s">
+      <c r="E111" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I111" s="8" t="s">
         <v>389</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H111" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I111" s="8" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D112" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C112" s="6" t="s">
+      <c r="E112" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I112" s="8" t="s">
         <v>389</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H112" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I112" s="8" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D113" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="C113" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>390</v>
-      </c>
       <c r="E113" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>9</v>
@@ -5450,21 +5449,21 @@
         <v>10</v>
       </c>
       <c r="I113" s="8" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="D114" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="E114" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>9</v>
@@ -5473,67 +5472,67 @@
         <v>10</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I115" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="G115" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="H115" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B117" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="D117" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="C117" s="6" t="s">
+      <c r="E117" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="F117" s="6" t="s">
         <v>405</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="F117" s="6" t="s">
-        <v>407</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>32</v>
@@ -5542,164 +5541,164 @@
         <v>26</v>
       </c>
       <c r="I117" s="10" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C118" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D118" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="E118" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D118" s="5" t="s">
+      <c r="F118" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="E118" s="11" t="s">
+      <c r="G118" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="H118" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I118" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="G118" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="H118" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I118" s="5" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B119" s="5" t="s">
+      <c r="D119" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E119" s="11" t="s">
         <v>417</v>
       </c>
-      <c r="C119" s="2" t="s">
+      <c r="F119" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D119" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="E119" s="11" t="s">
-        <v>419</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>420</v>
-      </c>
       <c r="G119" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H119" s="5" t="s">
         <v>26</v>
       </c>
       <c r="I119" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B120" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D120" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="E120" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="D120" s="5" t="s">
+      <c r="F120" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G120" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="H120" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I120" s="5" t="s">
         <v>424</v>
-      </c>
-      <c r="E120" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G120" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="H120" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I120" s="5" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B121" s="6"/>
       <c r="C121" s="5"/>
       <c r="D121" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E121" s="5"/>
       <c r="F121" s="5"/>
       <c r="G121" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H121" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I121" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="D122" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="C122" s="2" t="s">
+      <c r="E122" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="F122" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="D122" s="5" t="s">
+      <c r="G122" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H122" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I122" s="5" t="s">
         <v>433</v>
-      </c>
-      <c r="E122" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="G122" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H122" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I122" s="5" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="C123" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="D123" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="C123" s="2" t="s">
+      <c r="E123" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="F123" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="D123" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="E123" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>440</v>
       </c>
       <c r="G123" s="5" t="s">
         <v>32</v>
@@ -5708,162 +5707,162 @@
         <v>26</v>
       </c>
       <c r="I123" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="E125" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="C125" s="2" t="s">
+      <c r="G125" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I125" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H125" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I125" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="E126" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="C126" s="2" t="s">
+      <c r="G126" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I126" s="1" t="s">
         <v>452</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="G126" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H126" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I126" s="1" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D127" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="G127" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H127" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I127" s="1" t="s">
         <v>456</v>
-      </c>
-      <c r="D127" s="8" t="s">
-        <v>457</v>
-      </c>
-      <c r="G127" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H127" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I127" s="1" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="D128" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="F128" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="D128" s="6" t="s">
+      <c r="G128" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I128" s="1" t="s">
         <v>461</v>
-      </c>
-      <c r="F128" s="13" t="s">
-        <v>462</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H128" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I128" s="1" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="F129" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="B129" s="8" t="s">
+      <c r="G129" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I129" s="1" t="s">
         <v>465</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H129" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I129" s="1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B130" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="D130" s="6" t="s">
         <v>468</v>
       </c>
-      <c r="C130" s="6" t="s">
+      <c r="F130" s="15" t="s">
         <v>469</v>
       </c>
-      <c r="D130" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="F130" s="15" t="s">
-        <v>471</v>
-      </c>
       <c r="G130" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>10</v>
@@ -5871,224 +5870,224 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="B131" s="13" t="s">
+        <v>471</v>
+      </c>
+      <c r="C131" s="6" t="s">
         <v>472</v>
       </c>
-      <c r="B131" s="13" t="s">
+      <c r="D131" s="8" t="s">
         <v>473</v>
       </c>
-      <c r="C131" s="6" t="s">
+      <c r="E131" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="D131" s="8" t="s">
+      <c r="F131" s="13" t="s">
+        <v>473</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I131" s="1" t="s">
         <v>475</v>
-      </c>
-      <c r="E131" s="13" t="s">
-        <v>476</v>
-      </c>
-      <c r="F131" s="13" t="s">
-        <v>475</v>
-      </c>
-      <c r="G131" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H131" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I131" s="1" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B132" s="13" t="s">
+        <v>476</v>
+      </c>
+      <c r="C132" s="16" t="s">
+        <v>477</v>
+      </c>
+      <c r="D132" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="C132" s="16" t="s">
+      <c r="E132" s="13" t="s">
         <v>479</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>480</v>
-      </c>
-      <c r="E132" s="13" t="s">
-        <v>481</v>
       </c>
       <c r="F132" s="16"/>
       <c r="G132" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I132" s="17" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="13" t="s">
+        <v>480</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C133" s="6" t="s">
         <v>482</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="D133" s="8" t="s">
         <v>483</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="D133" s="8" t="s">
-        <v>485</v>
       </c>
       <c r="E133" s="13"/>
       <c r="F133" s="8" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H133" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C134" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="D134" s="16" t="s">
         <v>489</v>
-      </c>
-      <c r="C134" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="D134" s="16" t="s">
-        <v>491</v>
       </c>
       <c r="E134" s="13"/>
       <c r="G134" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H134" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F135" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H135" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I135" s="17" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D136" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="E136" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="F136" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="C136" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="E136" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>505</v>
-      </c>
       <c r="G136" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I136" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" s="12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F137" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H137" s="2" t="s">
         <v>26</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" s="14" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G138" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H138" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" s="18" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>32</v>
@@ -6097,21 +6096,21 @@
         <v>26</v>
       </c>
       <c r="I139" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C140" s="19" t="s">
+        <v>531</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="F140" s="2" t="s">
         <v>524</v>
-      </c>
-      <c r="C140" s="19" t="s">
-        <v>533</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>526</v>
       </c>
       <c r="G140" s="2" t="s">
         <v>32</v>
@@ -6120,34 +6119,34 @@
         <v>10</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="C141" s="19" t="s">
+        <v>532</v>
+      </c>
+      <c r="D141" s="19" t="s">
         <v>528</v>
       </c>
-      <c r="B141" s="8" t="s">
+      <c r="E141" s="8" t="s">
         <v>529</v>
-      </c>
-      <c r="C141" s="19" t="s">
-        <v>534</v>
-      </c>
-      <c r="D141" s="19" t="s">
-        <v>530</v>
-      </c>
-      <c r="E141" s="8" t="s">
-        <v>531</v>
       </c>
       <c r="F141" s="8"/>
       <c r="G141" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H141" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I141" s="20" t="s">
-        <v>532</v>
+      <c r="I141" s="8" t="s">
+        <v>530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed as.data.frame() issue with rolodex data
</commit_message>
<xml_diff>
--- a/data-raw/Rolodex.xlsx
+++ b/data-raw/Rolodex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\New Shiny Apps\Rolodex\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AA50BB-7753-4C21-A9EA-94807D8692C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C440EC1-29C9-4085-A27A-04FCC352CC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12570" yWindow="0" windowWidth="13120" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7610" yWindow="810" windowWidth="12980" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rolodex NEW" sheetId="1" r:id="rId1"/>
@@ -2666,7 +2666,7 @@
   <dimension ref="A1:I142"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6171,7 +6171,7 @@
       <c r="H142" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I142" t="s">
+      <c r="I142" s="2" t="s">
         <v>537</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed typos for RISSE
</commit_message>
<xml_diff>
--- a/data-raw/Rolodex.xlsx
+++ b/data-raw/Rolodex.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\New Shiny Apps\Rolodex\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69702A20-C47F-430E-93D8-443E5EF38646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC5A450-8CAC-4737-A34C-2B8C7CA7CAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1707,9 +1707,6 @@
     <t>Brainfuse provides real-time online tutoring, a comprehensive lesson library, and targeted diagnostic tests to support learners of all ages. Trusted by libraries, schools, and workforce centers across North America, Brainfuse connects users with expert instructors for personalized learning.</t>
   </si>
   <si>
-    <t>RISSE (Refgeee and Imigrant Support Services osf Emmaus)</t>
-  </si>
-  <si>
     <t>Title IX</t>
   </si>
   <si>
@@ -1828,6 +1825,9 @@
   </si>
   <si>
     <t>https://landing.brainfuse.com/saml.asp?oauth_consumer_key=33569B5A</t>
+  </si>
+  <si>
+    <t>RISSE (Refgeee and Immigrant Support Services of Emmaus)</t>
   </si>
 </sst>
 </file>
@@ -2797,7 +2797,7 @@
   <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156:XFD156"/>
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -5254,7 +5254,7 @@
         <v>10</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -5633,7 +5633,7 @@
         <v>10</v>
       </c>
       <c r="I115" s="12" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -6328,7 +6328,7 @@
         <v>539</v>
       </c>
       <c r="D144" s="11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>32</v>
@@ -6342,19 +6342,19 @@
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="2" t="s">
-        <v>541</v>
+        <v>580</v>
       </c>
       <c r="B145" s="19" t="s">
+        <v>546</v>
+      </c>
+      <c r="C145" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="D145" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="C145" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="D145" s="11" t="s">
+      <c r="E145" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>549</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>83</v>
@@ -6363,24 +6363,24 @@
         <v>10</v>
       </c>
       <c r="I145" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="2" t="s">
-        <v>541</v>
+        <v>580</v>
       </c>
       <c r="B146" s="19" t="s">
+        <v>546</v>
+      </c>
+      <c r="C146" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="D146" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="C146" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="D146" s="11" t="s">
+      <c r="E146" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>549</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>61</v>
@@ -6389,50 +6389,50 @@
         <v>10</v>
       </c>
       <c r="I146" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="2" t="s">
-        <v>541</v>
+        <v>580</v>
       </c>
       <c r="B147" s="19" t="s">
+        <v>546</v>
+      </c>
+      <c r="C147" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="D147" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="C147" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="D147" s="11" t="s">
+      <c r="E147" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="E147" s="2" t="s">
+      <c r="G147" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="H147" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I147" t="s">
         <v>549</v>
-      </c>
-      <c r="G147" s="2" t="s">
-        <v>576</v>
-      </c>
-      <c r="H147" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I147" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="148" spans="1:9">
       <c r="A148" s="2" t="s">
-        <v>541</v>
+        <v>580</v>
       </c>
       <c r="B148" s="19" t="s">
+        <v>546</v>
+      </c>
+      <c r="C148" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="D148" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="C148" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="D148" s="11" t="s">
+      <c r="E148" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>549</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>114</v>
@@ -6441,24 +6441,24 @@
         <v>10</v>
       </c>
       <c r="I148" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="149" spans="1:9">
       <c r="A149" s="2" t="s">
-        <v>541</v>
+        <v>580</v>
       </c>
       <c r="B149" s="19" t="s">
+        <v>546</v>
+      </c>
+      <c r="C149" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="D149" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="C149" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="D149" s="11" t="s">
+      <c r="E149" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>549</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>85</v>
@@ -6467,27 +6467,27 @@
         <v>10</v>
       </c>
       <c r="I149" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="150" spans="1:9">
       <c r="A150" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="C150" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="D150" s="11" t="s">
         <v>551</v>
       </c>
-      <c r="C150" s="11" t="s">
-        <v>572</v>
-      </c>
-      <c r="D150" s="11" t="s">
+      <c r="E150" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="E150" s="2" t="s">
+      <c r="F150" s="11" t="s">
         <v>553</v>
-      </c>
-      <c r="F150" s="11" t="s">
-        <v>554</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>126</v>
@@ -6496,18 +6496,18 @@
         <v>26</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="151" spans="1:9">
       <c r="A151" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B151" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="D151" s="11" t="s">
         <v>556</v>
-      </c>
-      <c r="D151" s="11" t="s">
-        <v>557</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>358</v>
@@ -6519,27 +6519,27 @@
         <v>10</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="152" spans="1:9">
       <c r="A152" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B152" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="C152" s="11" t="s">
+        <v>572</v>
+      </c>
+      <c r="D152" s="11" t="s">
         <v>559</v>
       </c>
-      <c r="C152" s="11" t="s">
-        <v>573</v>
-      </c>
-      <c r="D152" s="11" t="s">
+      <c r="E152" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E152" s="2" t="s">
+      <c r="F152" s="11" t="s">
         <v>561</v>
-      </c>
-      <c r="F152" s="11" t="s">
-        <v>562</v>
       </c>
       <c r="G152" s="2" t="s">
         <v>32</v>
@@ -6548,24 +6548,24 @@
         <v>26</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="153" spans="1:9">
       <c r="A153" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D153" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="E153" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>565</v>
       </c>
       <c r="G153" s="2" t="s">
         <v>78</v>
@@ -6574,27 +6574,27 @@
         <v>10</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="154" spans="1:9">
       <c r="A154" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D154" s="11" t="s">
+        <v>566</v>
+      </c>
+      <c r="E154" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="E154" s="2" t="s">
+      <c r="F154" s="11" t="s">
         <v>568</v>
-      </c>
-      <c r="F154" s="11" t="s">
-        <v>569</v>
       </c>
       <c r="G154" s="2" t="s">
         <v>32</v>
@@ -6603,7 +6603,7 @@
         <v>26</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -6626,7 +6626,7 @@
         <v>436</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H155" s="12" t="s">
         <v>26</v>
@@ -6649,7 +6649,7 @@
         <v>520</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H156" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
added Email feature (no link)
</commit_message>
<xml_diff>
--- a/data-raw/Rolodex.xlsx
+++ b/data-raw/Rolodex.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intra\Desktop\New Shiny Apps\Rolodex\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC5A450-8CAC-4737-A34C-2B8C7CA7CAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9869DD3A-8754-4FC6-9AAA-1173B2FE86CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1383,9 +1383,6 @@
     <t>https://www.albany.edu/isss/</t>
   </si>
   <si>
-    <t>ISSS@albany.edu</t>
-  </si>
-  <si>
     <t>Advising - workshops</t>
   </si>
   <si>
@@ -1828,6 +1825,9 @@
   </si>
   <si>
     <t>RISSE (Refgeee and Immigrant Support Services of Emmaus)</t>
+  </si>
+  <si>
+    <t>ISSS@albany.edu</t>
   </si>
 </sst>
 </file>
@@ -2796,8 +2796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+    <sheetView tabSelected="1" topLeftCell="B101" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5"/>
@@ -2929,7 +2929,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>175</v>
@@ -2953,7 +2953,7 @@
         <v>26</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3804,7 +3804,7 @@
         <v>26</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -4809,7 +4809,7 @@
         <v>26</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -5254,7 +5254,7 @@
         <v>10</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -5554,7 +5554,7 @@
         <v>84</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>407</v>
@@ -5633,7 +5633,7 @@
         <v>10</v>
       </c>
       <c r="I115" s="12" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -5671,7 +5671,7 @@
         <v>429</v>
       </c>
       <c r="E117" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>430</v>
@@ -5700,10 +5700,10 @@
         <v>435</v>
       </c>
       <c r="E118" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
+      </c>
+      <c r="F118" s="20" t="s">
+        <v>580</v>
       </c>
       <c r="G118" s="12" t="s">
         <v>32</v>
@@ -5712,21 +5712,21 @@
         <v>26</v>
       </c>
       <c r="I118" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>445</v>
-      </c>
       <c r="C119" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>358</v>
@@ -5738,21 +5738,21 @@
         <v>26</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C120" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="D120" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E120" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>449</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>51</v>
@@ -5761,21 +5761,21 @@
         <v>10</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="C121" s="2" t="s">
+      <c r="D121" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E121" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>449</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>78</v>
@@ -5784,18 +5784,18 @@
         <v>10</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="B122" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="D122" s="13" t="s">
         <v>452</v>
-      </c>
-      <c r="D122" s="13" t="s">
-        <v>453</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>114</v>
@@ -5804,21 +5804,21 @@
         <v>10</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" s="13" t="s">
+        <v>454</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="D123" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="D123" s="5" t="s">
+      <c r="F123" s="7" t="s">
         <v>457</v>
-      </c>
-      <c r="F123" s="7" t="s">
-        <v>458</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>114</v>
@@ -5827,18 +5827,18 @@
         <v>10</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B124" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="B124" s="13" t="s">
+      <c r="F124" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>462</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>114</v>
@@ -5847,24 +5847,24 @@
         <v>10</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="125" spans="1:9">
       <c r="A125" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="C125" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="C125" s="5" t="s">
+      <c r="D125" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="D125" s="5" t="s">
+      <c r="F125" s="16" t="s">
         <v>466</v>
-      </c>
-      <c r="F125" s="16" t="s">
-        <v>467</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>114</v>
@@ -5875,22 +5875,22 @@
     </row>
     <row r="126" spans="1:9">
       <c r="A126" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="B126" s="7" t="s">
         <v>468</v>
       </c>
-      <c r="B126" s="7" t="s">
+      <c r="C126" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="C126" s="5" t="s">
+      <c r="D126" s="13" t="s">
         <v>470</v>
       </c>
-      <c r="D126" s="13" t="s">
+      <c r="E126" s="7" t="s">
         <v>471</v>
       </c>
-      <c r="E126" s="7" t="s">
-        <v>472</v>
-      </c>
       <c r="F126" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>114</v>
@@ -5899,24 +5899,24 @@
         <v>10</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B127" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="C127" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="C127" s="8" t="s">
+      <c r="D127" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="D127" s="5" t="s">
+      <c r="E127" s="7" t="s">
         <v>476</v>
-      </c>
-      <c r="E127" s="7" t="s">
-        <v>477</v>
       </c>
       <c r="F127" s="8"/>
       <c r="G127" s="1" t="s">
@@ -5926,25 +5926,25 @@
         <v>10</v>
       </c>
       <c r="I127" s="17" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="128" spans="1:9">
       <c r="A128" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="B128" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="C128" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="C128" s="5" t="s">
+      <c r="D128" s="13" t="s">
         <v>480</v>
-      </c>
-      <c r="D128" s="13" t="s">
-        <v>481</v>
       </c>
       <c r="E128" s="7"/>
       <c r="F128" s="13" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>61</v>
@@ -5953,21 +5953,21 @@
         <v>10</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="129" spans="1:9">
       <c r="A129" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="C129" s="5" t="s">
         <v>485</v>
       </c>
-      <c r="C129" s="5" t="s">
+      <c r="D129" s="8" t="s">
         <v>486</v>
-      </c>
-      <c r="D129" s="8" t="s">
-        <v>487</v>
       </c>
       <c r="E129" s="7"/>
       <c r="G129" s="1" t="s">
@@ -5977,21 +5977,21 @@
         <v>10</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="130" spans="1:9">
       <c r="A130" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B130" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="D130" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="D130" s="2" t="s">
-        <v>498</v>
-      </c>
       <c r="E130" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F130" s="5" t="s">
         <v>49</v>
@@ -6003,27 +6003,27 @@
         <v>26</v>
       </c>
       <c r="I130" s="17" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="131" spans="1:9">
       <c r="A131" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>497</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>270</v>
       </c>
       <c r="D131" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="F131" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>499</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>61</v>
@@ -6032,21 +6032,21 @@
         <v>26</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="132" spans="1:9">
       <c r="A132" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D132" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E132" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>504</v>
       </c>
       <c r="F132" s="5" t="s">
         <v>49</v>
@@ -6058,21 +6058,21 @@
         <v>26</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="133" spans="1:9">
       <c r="A133" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>51</v>
@@ -6081,18 +6081,18 @@
         <v>10</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="18" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>32</v>
@@ -6101,21 +6101,21 @@
         <v>26</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="135" spans="1:9">
       <c r="A135" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C135" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="D135" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="C135" s="11" t="s">
-        <v>527</v>
-      </c>
-      <c r="D135" s="2" t="s">
+      <c r="F135" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>32</v>
@@ -6124,24 +6124,24 @@
         <v>10</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="136" spans="1:9">
       <c r="A136" s="13" t="s">
+        <v>521</v>
+      </c>
+      <c r="B136" s="13" t="s">
         <v>522</v>
       </c>
-      <c r="B136" s="13" t="s">
+      <c r="C136" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="D136" s="11" t="s">
         <v>523</v>
       </c>
-      <c r="C136" s="11" t="s">
-        <v>528</v>
-      </c>
-      <c r="D136" s="11" t="s">
+      <c r="E136" s="13" t="s">
         <v>524</v>
-      </c>
-      <c r="E136" s="13" t="s">
-        <v>525</v>
       </c>
       <c r="F136" s="13"/>
       <c r="G136" s="13" t="s">
@@ -6151,15 +6151,15 @@
         <v>10</v>
       </c>
       <c r="I136" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="137" spans="1:9">
       <c r="A137" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>345</v>
@@ -6168,15 +6168,15 @@
         <v>10</v>
       </c>
       <c r="I137" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="138" spans="1:9">
       <c r="A138" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="D138" s="11" t="s">
         <v>534</v>
-      </c>
-      <c r="D138" s="11" t="s">
-        <v>535</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>61</v>
@@ -6185,25 +6185,25 @@
         <v>10</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G139" s="1" t="s">
         <v>104</v>
@@ -6212,25 +6212,25 @@
         <v>10</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="140" spans="1:9">
       <c r="A140" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>95</v>
@@ -6239,25 +6239,25 @@
         <v>10</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="141" spans="1:9">
       <c r="A141" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>51</v>
@@ -6266,25 +6266,25 @@
         <v>10</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="142" spans="1:9">
       <c r="A142" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>78</v>
@@ -6293,25 +6293,25 @@
         <v>10</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="143" spans="1:9">
       <c r="A143" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>85</v>
@@ -6320,15 +6320,15 @@
         <v>10</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="144" spans="1:9">
       <c r="A144" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D144" s="11" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>32</v>
@@ -6337,24 +6337,24 @@
         <v>10</v>
       </c>
       <c r="I144" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B145" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="C145" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="D145" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="C145" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="D145" s="11" t="s">
+      <c r="E145" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>548</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>83</v>
@@ -6363,24 +6363,24 @@
         <v>10</v>
       </c>
       <c r="I145" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B146" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="C146" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="D146" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="C146" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="D146" s="11" t="s">
+      <c r="E146" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>548</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>61</v>
@@ -6389,50 +6389,50 @@
         <v>10</v>
       </c>
       <c r="I146" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="147" spans="1:9">
       <c r="A147" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B147" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="C147" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="D147" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="C147" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="D147" s="11" t="s">
+      <c r="E147" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="E147" s="2" t="s">
+      <c r="G147" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="H147" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I147" t="s">
         <v>548</v>
-      </c>
-      <c r="G147" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="H147" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I147" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="148" spans="1:9">
       <c r="A148" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B148" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="C148" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="D148" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="C148" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="D148" s="11" t="s">
+      <c r="E148" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>548</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>114</v>
@@ -6441,24 +6441,24 @@
         <v>10</v>
       </c>
       <c r="I148" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="149" spans="1:9">
       <c r="A149" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B149" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="C149" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="D149" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="C149" s="11" t="s">
-        <v>570</v>
-      </c>
-      <c r="D149" s="11" t="s">
+      <c r="E149" s="2" t="s">
         <v>547</v>
-      </c>
-      <c r="E149" s="2" t="s">
-        <v>548</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>85</v>
@@ -6467,27 +6467,27 @@
         <v>10</v>
       </c>
       <c r="I149" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="150" spans="1:9">
       <c r="A150" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C150" s="11" t="s">
+        <v>570</v>
+      </c>
+      <c r="D150" s="11" t="s">
         <v>550</v>
       </c>
-      <c r="C150" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="D150" s="11" t="s">
+      <c r="E150" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="E150" s="2" t="s">
+      <c r="F150" s="11" t="s">
         <v>552</v>
-      </c>
-      <c r="F150" s="11" t="s">
-        <v>553</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>126</v>
@@ -6496,18 +6496,18 @@
         <v>26</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="151" spans="1:9">
       <c r="A151" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B151" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="D151" s="11" t="s">
         <v>555</v>
-      </c>
-      <c r="D151" s="11" t="s">
-        <v>556</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>358</v>
@@ -6519,27 +6519,27 @@
         <v>10</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="152" spans="1:9">
       <c r="A152" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B152" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="C152" s="11" t="s">
+        <v>571</v>
+      </c>
+      <c r="D152" s="11" t="s">
         <v>558</v>
       </c>
-      <c r="C152" s="11" t="s">
-        <v>572</v>
-      </c>
-      <c r="D152" s="11" t="s">
+      <c r="E152" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="E152" s="2" t="s">
+      <c r="F152" s="11" t="s">
         <v>560</v>
-      </c>
-      <c r="F152" s="11" t="s">
-        <v>561</v>
       </c>
       <c r="G152" s="2" t="s">
         <v>32</v>
@@ -6548,24 +6548,24 @@
         <v>26</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="153" spans="1:9">
       <c r="A153" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D153" s="11" t="s">
+        <v>562</v>
+      </c>
+      <c r="E153" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>564</v>
       </c>
       <c r="G153" s="2" t="s">
         <v>78</v>
@@ -6574,27 +6574,27 @@
         <v>10</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="154" spans="1:9">
       <c r="A154" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D154" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="E154" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="E154" s="2" t="s">
+      <c r="F154" s="11" t="s">
         <v>567</v>
-      </c>
-      <c r="F154" s="11" t="s">
-        <v>568</v>
       </c>
       <c r="G154" s="2" t="s">
         <v>32</v>
@@ -6603,7 +6603,7 @@
         <v>26</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -6620,42 +6620,42 @@
         <v>435</v>
       </c>
       <c r="E155" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="F155" s="2" t="s">
-        <v>436</v>
+        <v>438</v>
+      </c>
+      <c r="F155" s="20" t="s">
+        <v>580</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H155" s="12" t="s">
         <v>26</v>
       </c>
       <c r="I155" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="156" spans="1:9">
       <c r="A156" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="D156" s="20" t="s">
         <v>518</v>
       </c>
-      <c r="C156" s="11" t="s">
-        <v>527</v>
-      </c>
-      <c r="D156" s="20" t="s">
+      <c r="F156" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="F156" s="2" t="s">
+      <c r="G156" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I156" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="G156" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="H156" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I156" s="1" t="s">
-        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -6774,8 +6774,10 @@
     <hyperlink ref="C154" r:id="rId109" xr:uid="{7C2DE1D7-47ED-40CF-937D-415B2488F028}"/>
     <hyperlink ref="C156" r:id="rId110" xr:uid="{B28590EE-4458-4CAE-AE78-9975E73BC873}"/>
     <hyperlink ref="D156" r:id="rId111" xr:uid="{1E66DBCC-AB5E-4E32-804B-D7193FA752EE}"/>
+    <hyperlink ref="F118" r:id="rId112" xr:uid="{7369515B-3200-4C5D-8DBA-683E7EA7089D}"/>
+    <hyperlink ref="F155" r:id="rId113" xr:uid="{F7A76B19-1F37-4DF5-BD65-E0CE94052793}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId112"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId114"/>
 </worksheet>
 </file>
</xml_diff>